<commit_message>
Lin EIS Sens Study - Warburg Params
</commit_message>
<xml_diff>
--- a/GEN2_XLSX_CELLDEFS/cellLMO-P2DM.xlsx
+++ b/GEN2_XLSX_CELLDEFS/cellLMO-P2DM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10719"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uccsoffice365-my.sharepoint.com/personal/whileman_uccs_edu/Documents/MasterThesis/WesH-MasterThesis/assets/GEN2_XLSX_CELLDEFS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{3CA435F3-D629-5A49-836A-AF86D68F6E8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD58BA05-91FF-2C44-9A27-48E8A418AB2B}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{3CA435F3-D629-5A49-836A-AF86D68F6E8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8102E61E-A884-A240-8BA5-582B7210D36A}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" tabRatio="629" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15220" yWindow="500" windowWidth="22800" windowHeight="16360" tabRatio="629" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="16" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="191">
   <si>
     <t>Code Name</t>
   </si>
@@ -660,6 +660,27 @@
   </si>
   <si>
     <t>n_\mathrm{f}</t>
+  </si>
+  <si>
+    <t>Solid-phase diffusivity CPE-integrator time const.</t>
+  </si>
+  <si>
+    <t>tauF</t>
+  </si>
+  <si>
+    <t>\tau_\mathrm{f}</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>Empirical multiplicity of solid diffusivity</t>
+  </si>
+  <si>
+    <t>mD</t>
+  </si>
+  <si>
+    <t>m_\mathrm{D}</t>
   </si>
 </sst>
 </file>
@@ -2213,6 +2234,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2538,15 +2563,15 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G71"/>
+  <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="42.6640625" customWidth="1"/>
     <col min="3" max="3" width="16.1640625" customWidth="1"/>
     <col min="4" max="4" width="20.83203125" customWidth="1"/>
@@ -2555,7 +2580,7 @@
     <col min="7" max="7" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="35" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>93</v>
       </c>
@@ -2578,7 +2603,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="43" t="s">
         <v>7</v>
       </c>
@@ -3547,15 +3572,15 @@
     </row>
     <row r="58" spans="2:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="6" t="s">
-        <v>15</v>
+        <v>188</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>68</v>
+        <v>189</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="E58" s="22">
+        <v>190</v>
+      </c>
+      <c r="E58" s="37">
         <v>1</v>
       </c>
       <c r="F58" s="22">
@@ -3567,192 +3592,232 @@
     </row>
     <row r="59" spans="2:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B59" s="6" t="s">
-        <v>140</v>
+        <v>15</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="E59" s="38" t="s">
-        <v>144</v>
-      </c>
-      <c r="F59" s="39">
+        <v>183</v>
+      </c>
+      <c r="E59" s="22">
+        <v>1</v>
+      </c>
+      <c r="F59" s="22">
         <v>0</v>
       </c>
       <c r="G59" s="8" t="s">
-        <v>147</v>
+        <v>14</v>
       </c>
     </row>
     <row r="60" spans="2:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B60" s="6" t="s">
-        <v>141</v>
+        <v>184</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>21</v>
+        <v>185</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="E60" s="38" t="s">
-        <v>145</v>
-      </c>
-      <c r="F60" s="39">
+        <v>186</v>
+      </c>
+      <c r="E60" s="22">
+        <v>100</v>
+      </c>
+      <c r="F60" s="22">
         <v>0</v>
       </c>
       <c r="G60" s="8" t="s">
-        <v>14</v>
+        <v>187</v>
       </c>
     </row>
     <row r="61" spans="2:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B61" s="6" t="s">
-        <v>114</v>
+        <v>140</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="E61" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="F61" s="22">
+        <v>160</v>
+      </c>
+      <c r="E61" s="38" t="s">
+        <v>144</v>
+      </c>
+      <c r="F61" s="39">
         <v>0</v>
       </c>
       <c r="G61" s="8" t="s">
-        <v>121</v>
+        <v>147</v>
       </c>
     </row>
     <row r="62" spans="2:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B62" s="6" t="s">
-        <v>11</v>
+        <v>141</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>67</v>
+        <v>21</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="E62" s="22">
-        <v>0.22</v>
-      </c>
-      <c r="F62" s="22">
+        <v>163</v>
+      </c>
+      <c r="E62" s="38" t="s">
+        <v>145</v>
+      </c>
+      <c r="F62" s="39">
         <v>0</v>
       </c>
       <c r="G62" s="8" t="s">
-        <v>122</v>
+        <v>14</v>
       </c>
     </row>
     <row r="63" spans="2:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B63" s="6" t="s">
-        <v>13</v>
+        <v>114</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>69</v>
+        <v>24</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="E63" s="22">
-        <v>1</v>
+        <v>165</v>
+      </c>
+      <c r="E63" s="9">
+        <v>0.02</v>
       </c>
       <c r="F63" s="22">
         <v>0</v>
       </c>
       <c r="G63" s="8" t="s">
-        <v>14</v>
+        <v>121</v>
       </c>
     </row>
     <row r="64" spans="2:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B64" s="6" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E64" s="22">
-        <v>0</v>
+        <v>0.22</v>
       </c>
       <c r="F64" s="22">
         <v>0</v>
       </c>
       <c r="G64" s="8" t="s">
-        <v>94</v>
+        <v>122</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B65" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="E65" s="33">
-        <v>0</v>
+        <v>167</v>
+      </c>
+      <c r="E65" s="22">
+        <v>1</v>
       </c>
       <c r="F65" s="22">
         <v>0</v>
       </c>
       <c r="G65" s="8" t="s">
-        <v>121</v>
+        <v>14</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B66" s="6" t="s">
-        <v>115</v>
+        <v>22</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>116</v>
+        <v>25</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E66" s="22">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="F66" s="22">
         <v>0</v>
       </c>
       <c r="G66" s="8" t="s">
-        <v>14</v>
+        <v>94</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B67" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="E67" s="33">
+        <v>0</v>
+      </c>
+      <c r="F67" s="22">
+        <v>0</v>
+      </c>
+      <c r="G67" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B68" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="E68" s="22">
+        <v>1.5</v>
+      </c>
+      <c r="F68" s="22">
+        <v>0</v>
+      </c>
+      <c r="G68" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B69" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="C67" s="6" t="s">
+      <c r="C69" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="D67" s="6" t="s">
+      <c r="D69" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="E67" s="22">
+      <c r="E69" s="22">
         <v>1.5</v>
       </c>
-      <c r="F67" s="22">
-        <v>0</v>
-      </c>
-      <c r="G67" s="8" t="s">
+      <c r="F69" s="22">
+        <v>0</v>
+      </c>
+      <c r="G69" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
+    <row r="70" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="71" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="B44:G44"/>

</xml_diff>

<commit_message>
Updates to fix linEIS regression
</commit_message>
<xml_diff>
--- a/GEN2_XLSX_CELLDEFS/cellLMO-P2DM.xlsx
+++ b/GEN2_XLSX_CELLDEFS/cellLMO-P2DM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uccsoffice365-my.sharepoint.com/personal/whileman_uccs_edu/Documents/MasterThesis/WesH-MasterThesis/assets/GEN2_XLSX_CELLDEFS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CLiMB\LMB_Toolkit\GEN2_XLSX_CELLDEFS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{3CA435F3-D629-5A49-836A-AF86D68F6E8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8102E61E-A884-A240-8BA5-582B7210D36A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48DA3A2-6430-4CFE-B11E-8780DC6DFE6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15220" yWindow="500" windowWidth="22800" windowHeight="16360" tabRatio="629" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1275" yWindow="780" windowWidth="25995" windowHeight="15015" tabRatio="629" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="16" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="198">
   <si>
     <t>Code Name</t>
   </si>
@@ -674,20 +674,41 @@
     <t>s</t>
   </si>
   <si>
-    <t>Empirical multiplicity of solid diffusivity</t>
-  </si>
-  <si>
-    <t>mD</t>
-  </si>
-  <si>
-    <t>m_\mathrm{D}</t>
+    <t>Package Parameters</t>
+  </si>
+  <si>
+    <t>Tab resistance</t>
+  </si>
+  <si>
+    <t>R0</t>
+  </si>
+  <si>
+    <t>R_0</t>
+  </si>
+  <si>
+    <t>Ohm</t>
+  </si>
+  <si>
+    <t>Series inductance</t>
+  </si>
+  <si>
+    <t>L0</t>
+  </si>
+  <si>
+    <t>L_0</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>#pkg[Package]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="14">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1532,7 +1553,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1682,6 +1703,10 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="5" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="491">
@@ -2234,10 +2259,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2563,24 +2584,24 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G73"/>
+  <dimension ref="A1:G77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="42.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.1640625" customWidth="1"/>
-    <col min="4" max="4" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="9.25" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="42.625" customWidth="1"/>
+    <col min="3" max="3" width="16.125" customWidth="1"/>
+    <col min="4" max="4" width="20.875" customWidth="1"/>
     <col min="5" max="5" width="73.5" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12.625" customWidth="1"/>
+    <col min="7" max="7" width="10.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="35" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="35.1" hidden="1" customHeight="1" thickBot="1">
       <c r="A1" t="s">
         <v>93</v>
       </c>
@@ -2603,7 +2624,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="36" hidden="1" customHeight="1">
       <c r="B2" s="43" t="s">
         <v>7</v>
       </c>
@@ -2613,7 +2634,7 @@
       <c r="F2" s="44"/>
       <c r="G2" s="45"/>
     </row>
-    <row r="3" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="16.5" thickBot="1">
       <c r="B3" s="46"/>
       <c r="C3" s="47"/>
       <c r="D3" s="47"/>
@@ -2621,8 +2642,8 @@
       <c r="F3" s="47"/>
       <c r="G3" s="48"/>
     </row>
-    <row r="4" spans="1:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:7" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="12" customHeight="1" thickBot="1"/>
+    <row r="5" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
       <c r="B5" s="40" t="s">
         <v>5</v>
       </c>
@@ -2632,7 +2653,7 @@
       <c r="F5" s="41"/>
       <c r="G5" s="42"/>
     </row>
-    <row r="6" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="32" t="s">
         <v>91</v>
       </c>
@@ -2655,7 +2676,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="15.95" customHeight="1">
       <c r="B7" s="4" t="s">
         <v>86</v>
       </c>
@@ -2675,7 +2696,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="15.95" customHeight="1">
       <c r="B8" s="10" t="s">
         <v>87</v>
       </c>
@@ -2695,15 +2716,15 @@
         <v>153</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A9" t="s">
         <v>92</v>
       </c>
       <c r="G9" s="20"/>
     </row>
-    <row r="10" spans="1:7" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
       <c r="B10" s="40" t="s">
-        <v>8</v>
+        <v>188</v>
       </c>
       <c r="C10" s="41"/>
       <c r="D10" s="41"/>
@@ -2711,9 +2732,9 @@
       <c r="F10" s="41"/>
       <c r="G10" s="42"/>
     </row>
-    <row r="11" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A11" s="32" t="s">
-        <v>80</v>
+        <v>197</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>1</v>
@@ -2734,1034 +2755,1013 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="B12" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="E12" s="23">
+        <v>0.1</v>
+      </c>
+      <c r="F12" s="22">
+        <v>0</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="B13" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="E13" s="52">
+        <v>1E-8</v>
+      </c>
+      <c r="F13" s="22">
+        <v>0</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1">
+      <c r="A14" t="s">
+        <v>92</v>
+      </c>
+      <c r="G14" s="20"/>
+    </row>
+    <row r="15" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
+      <c r="B15" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="42"/>
+    </row>
+    <row r="16" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A16" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B17" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C17" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D17" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E12" s="23">
+      <c r="E17" s="23">
         <f>0.0064</f>
         <v>6.4000000000000003E-3</v>
       </c>
-      <c r="F12" s="22">
-        <v>0</v>
-      </c>
-      <c r="G12" s="7" t="s">
+      <c r="F17" s="22">
+        <v>0</v>
+      </c>
+      <c r="G17" s="7" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="5" t="s">
+    <row r="18" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B18" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C18" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D18" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="E13" s="23">
+      <c r="E18" s="23">
         <v>1000</v>
       </c>
-      <c r="F13" s="22">
-        <v>0</v>
-      </c>
-      <c r="G13" s="8" t="s">
+      <c r="F18" s="22">
+        <v>0</v>
+      </c>
+      <c r="G18" s="8" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="6" t="s">
+    <row r="19" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B19" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C19" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D19" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="E14" s="22">
+      <c r="E19" s="22">
         <v>0.8</v>
       </c>
-      <c r="F14" s="22">
-        <v>0</v>
-      </c>
-      <c r="G14" s="8" t="s">
+      <c r="F19" s="22">
+        <v>0</v>
+      </c>
+      <c r="G19" s="8" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="6" t="s">
+    <row r="20" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B20" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C20" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D20" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="E15" s="33">
+      <c r="E20" s="33">
         <v>2.5800000000000002E-9</v>
       </c>
-      <c r="F15" s="22">
-        <v>0</v>
-      </c>
-      <c r="G15" s="8" t="s">
+      <c r="F20" s="22">
+        <v>0</v>
+      </c>
+      <c r="G20" s="8" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="6" t="s">
+    <row r="21" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B21" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C21" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D21" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="E16" s="22">
+      <c r="E21" s="22">
         <v>0.4</v>
       </c>
-      <c r="F16" s="22">
-        <v>0</v>
-      </c>
-      <c r="G16" s="8" t="s">
+      <c r="F21" s="22">
+        <v>0</v>
+      </c>
+      <c r="G21" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="6" t="s">
+    <row r="22" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B22" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C22" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D22" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="E17" s="22">
+      <c r="E22" s="22">
         <v>3</v>
       </c>
-      <c r="F17" s="22">
-        <v>0</v>
-      </c>
-      <c r="G17" s="8" t="s">
+      <c r="F22" s="22">
+        <v>0</v>
+      </c>
+      <c r="G22" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="6" t="s">
+    <row r="23" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B23" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C23" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D23" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="E18" s="22">
+      <c r="E23" s="22">
         <v>298.14999999999998</v>
       </c>
-      <c r="F18" s="22">
-        <v>0</v>
-      </c>
-      <c r="G18" s="8" t="s">
+      <c r="F23" s="22">
+        <v>0</v>
+      </c>
+      <c r="G23" s="8" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="24" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1">
+      <c r="A24" t="s">
         <v>92</v>
       </c>
-      <c r="G19" s="20"/>
-    </row>
-    <row r="20" spans="1:7" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="40" t="s">
+      <c r="G24" s="20"/>
+    </row>
+    <row r="25" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
+      <c r="B25" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="42"/>
-    </row>
-    <row r="21" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="32" t="s">
+      <c r="C25" s="41"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="41"/>
+      <c r="F25" s="41"/>
+      <c r="G25" s="42"/>
+    </row>
+    <row r="26" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A26" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B26" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D21" s="11" t="s">
+      <c r="C26" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E26" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F26" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G26" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="6" t="s">
+    <row r="27" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B27" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C27" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D27" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="E22" s="33">
+      <c r="E27" s="33">
         <v>3.5000000000000002E-8</v>
       </c>
-      <c r="F22" s="22">
-        <v>0</v>
-      </c>
-      <c r="G22" s="8" t="s">
+      <c r="F27" s="22">
+        <v>0</v>
+      </c>
+      <c r="G27" s="8" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="6" t="s">
+    <row r="28" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B28" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C28" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D28" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="E23" s="33">
+      <c r="E28" s="33">
         <v>76900</v>
       </c>
-      <c r="F23" s="22">
-        <v>0</v>
-      </c>
-      <c r="G23" s="8" t="s">
+      <c r="F28" s="22">
+        <v>0</v>
+      </c>
+      <c r="G28" s="8" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="6" t="s">
+    <row r="29" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B29" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C29" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D29" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="E24" s="9">
+      <c r="E29" s="9">
         <v>0.7</v>
       </c>
-      <c r="F24" s="22">
-        <v>0</v>
-      </c>
-      <c r="G24" s="8" t="s">
+      <c r="F29" s="22">
+        <v>0</v>
+      </c>
+      <c r="G29" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="6" t="s">
+    <row r="30" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B30" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C30" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D30" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E25" s="22">
+      <c r="E30" s="22">
         <v>1</v>
       </c>
-      <c r="F25" s="22">
-        <v>0</v>
-      </c>
-      <c r="G25" s="8" t="s">
+      <c r="F30" s="22">
+        <v>0</v>
+      </c>
+      <c r="G30" s="8" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="6" t="s">
+    <row r="31" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B31" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C31" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D31" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="E26" s="9">
+      <c r="E31" s="9">
         <v>0.02</v>
       </c>
-      <c r="F26" s="22">
-        <v>0</v>
-      </c>
-      <c r="G26" s="34" t="s">
+      <c r="F31" s="22">
+        <v>0</v>
+      </c>
+      <c r="G31" s="34" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="6" t="s">
+    <row r="32" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B32" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C32" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D32" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="E27" s="22">
+      <c r="E32" s="22">
         <v>0.19800000000000001</v>
       </c>
-      <c r="F27" s="22">
-        <v>0</v>
-      </c>
-      <c r="G27" s="8" t="s">
+      <c r="F32" s="22">
+        <v>0</v>
+      </c>
+      <c r="G32" s="8" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="6" t="s">
+    <row r="33" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B33" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C33" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D33" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="E28" s="22">
+      <c r="E33" s="22">
         <v>1</v>
       </c>
-      <c r="F28" s="22">
-        <v>0</v>
-      </c>
-      <c r="G28" s="8" t="s">
+      <c r="F33" s="22">
+        <v>0</v>
+      </c>
+      <c r="G33" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="6" t="s">
+    <row r="34" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B34" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C34" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D34" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="E29" s="22">
-        <v>0</v>
-      </c>
-      <c r="F29" s="22">
-        <v>0</v>
-      </c>
-      <c r="G29" s="8" t="s">
+      <c r="E34" s="22">
+        <v>0</v>
+      </c>
+      <c r="F34" s="22">
+        <v>0</v>
+      </c>
+      <c r="G34" s="8" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="6" t="s">
+    <row r="35" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B35" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C35" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D35" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="E30" s="33">
-        <v>0</v>
-      </c>
-      <c r="F30" s="22">
-        <v>0</v>
-      </c>
-      <c r="G30" s="34" t="s">
+      <c r="E35" s="33">
+        <v>0</v>
+      </c>
+      <c r="F35" s="22">
+        <v>0</v>
+      </c>
+      <c r="G35" s="34" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="36" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1">
+      <c r="A36" t="s">
         <v>92</v>
       </c>
-      <c r="G31" s="20"/>
-    </row>
-    <row r="32" spans="1:7" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="49" t="s">
+      <c r="G36" s="20"/>
+    </row>
+    <row r="37" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
+      <c r="B37" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="C32" s="50"/>
-      <c r="D32" s="50"/>
-      <c r="E32" s="50"/>
-      <c r="F32" s="50"/>
-      <c r="G32" s="51"/>
-    </row>
-    <row r="33" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="C37" s="50"/>
+      <c r="D37" s="50"/>
+      <c r="E37" s="50"/>
+      <c r="F37" s="50"/>
+      <c r="G37" s="51"/>
+    </row>
+    <row r="38" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A38" t="s">
         <v>83</v>
       </c>
-      <c r="B33" s="24" t="s">
+      <c r="B38" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C33" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="D33" s="25" t="s">
+      <c r="C38" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="E33" s="25" t="s">
+      <c r="E38" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="F33" s="26" t="s">
+      <c r="F38" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="G33" s="27" t="s">
+      <c r="G38" s="27" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="28" t="s">
+    <row r="39" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B39" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="C34" s="29" t="s">
+      <c r="C39" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="D34" s="29" t="s">
+      <c r="D39" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="E34" s="35">
+      <c r="E39" s="35">
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="F34" s="30">
-        <v>0</v>
-      </c>
-      <c r="G34" s="31" t="s">
+      <c r="F39" s="30">
+        <v>0</v>
+      </c>
+      <c r="G39" s="31" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="28" t="s">
+    <row r="40" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B40" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="C35" s="29" t="s">
+      <c r="C40" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="D35" s="29" t="s">
+      <c r="D40" s="29" t="s">
         <v>172</v>
       </c>
-      <c r="E35" s="30">
+      <c r="E40" s="30">
         <v>0.21</v>
       </c>
-      <c r="F35" s="30">
-        <v>0</v>
-      </c>
-      <c r="G35" s="31" t="s">
+      <c r="F40" s="30">
+        <v>0</v>
+      </c>
+      <c r="G40" s="31" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="28" t="s">
+    <row r="41" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B41" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="C36" s="29" t="s">
+      <c r="C41" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D41" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="E36" s="30">
+      <c r="E41" s="30">
         <v>1.5</v>
       </c>
-      <c r="F36" s="30">
-        <v>0</v>
-      </c>
-      <c r="G36" s="31" t="s">
+      <c r="F41" s="30">
+        <v>0</v>
+      </c>
+      <c r="G41" s="31" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="42" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1">
+      <c r="A42" t="s">
         <v>92</v>
       </c>
-      <c r="G37" s="20"/>
-    </row>
-    <row r="38" spans="1:7" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="40" t="s">
+      <c r="G42" s="20"/>
+    </row>
+    <row r="43" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
+      <c r="B43" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="C38" s="41"/>
-      <c r="D38" s="41"/>
-      <c r="E38" s="41"/>
-      <c r="F38" s="41"/>
-      <c r="G38" s="42"/>
-    </row>
-    <row r="39" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="32" t="s">
+      <c r="C43" s="41"/>
+      <c r="D43" s="41"/>
+      <c r="E43" s="41"/>
+      <c r="F43" s="41"/>
+      <c r="G43" s="42"/>
+    </row>
+    <row r="44" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A44" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="B39" s="11" t="s">
+      <c r="B44" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C39" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D39" s="11" t="s">
+      <c r="C44" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D44" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="E39" s="11" t="s">
+      <c r="E44" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="F44" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G39" s="3" t="s">
+      <c r="G44" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="6" t="s">
+    <row r="45" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B45" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C45" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="D40" s="29" t="s">
+      <c r="D45" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="E40" s="36">
+      <c r="E45" s="36">
         <v>2.5000000000000001E-5</v>
       </c>
-      <c r="F40" s="22">
-        <v>0</v>
-      </c>
-      <c r="G40" s="8" t="s">
+      <c r="F45" s="22">
+        <v>0</v>
+      </c>
+      <c r="G45" s="8" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="6" t="s">
+    <row r="46" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B46" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C46" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D41" s="29" t="s">
+      <c r="D46" s="29" t="s">
         <v>172</v>
       </c>
-      <c r="E41" s="22">
+      <c r="E46" s="22">
         <v>0.41</v>
       </c>
-      <c r="F41" s="22">
-        <v>0</v>
-      </c>
-      <c r="G41" s="8" t="s">
+      <c r="F46" s="22">
+        <v>0</v>
+      </c>
+      <c r="G46" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="6" t="s">
+    <row r="47" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B47" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C47" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="D47" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="E42" s="22">
+      <c r="E47" s="22">
         <v>1.5</v>
       </c>
-      <c r="F42" s="22">
-        <v>0</v>
-      </c>
-      <c r="G42" s="8" t="s">
+      <c r="F47" s="22">
+        <v>0</v>
+      </c>
+      <c r="G47" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="48" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1">
+      <c r="A48" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="40" t="s">
+    <row r="49" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
+      <c r="B49" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="C44" s="41"/>
-      <c r="D44" s="41"/>
-      <c r="E44" s="41"/>
-      <c r="F44" s="41"/>
-      <c r="G44" s="42"/>
-    </row>
-    <row r="45" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="32" t="s">
+      <c r="C49" s="41"/>
+      <c r="D49" s="41"/>
+      <c r="E49" s="41"/>
+      <c r="F49" s="41"/>
+      <c r="G49" s="42"/>
+    </row>
+    <row r="50" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A50" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="B45" s="11" t="s">
+      <c r="B50" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C45" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D45" s="11" t="s">
+      <c r="C50" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D50" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="E45" s="11" t="s">
+      <c r="E50" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F45" s="2" t="s">
+      <c r="F50" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G45" s="3" t="s">
+      <c r="G50" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="6" t="s">
+    <row r="51" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B51" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C51" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D46" s="6" t="s">
+      <c r="D51" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="E46" s="21" t="s">
+      <c r="E51" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="F46" s="9">
-        <v>0</v>
-      </c>
-      <c r="G46" s="7" t="s">
+      <c r="F51" s="9">
+        <v>0</v>
+      </c>
+      <c r="G51" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="6" t="s">
+    <row r="52" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B52" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="C52" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="D52" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="E47" s="21" t="s">
+      <c r="E52" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="F47" s="9">
-        <v>0</v>
-      </c>
-      <c r="G47" s="7" t="s">
+      <c r="F52" s="9">
+        <v>0</v>
+      </c>
+      <c r="G52" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="6" t="s">
+    <row r="53" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B53" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C53" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D48" s="6" t="s">
+      <c r="D53" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="E48" s="21" t="s">
+      <c r="E53" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="F48" s="9">
-        <v>0</v>
-      </c>
-      <c r="G48" s="7" t="s">
+      <c r="F53" s="9">
+        <v>0</v>
+      </c>
+      <c r="G53" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="2:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="6" t="s">
+    <row r="54" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B54" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="C49" s="6" t="s">
+      <c r="C54" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="D49" s="6" t="s">
+      <c r="D54" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="E49" s="36">
+      <c r="E54" s="36">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="F49" s="22">
-        <v>0</v>
-      </c>
-      <c r="G49" s="7" t="s">
+      <c r="F54" s="22">
+        <v>0</v>
+      </c>
+      <c r="G54" s="7" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="50" spans="2:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="6" t="s">
+    <row r="55" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B55" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="C50" s="6" t="s">
+      <c r="C55" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="D50" s="6" t="s">
+      <c r="D55" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="E50" s="36">
+      <c r="E55" s="36">
         <v>3.9999999999999998E-6</v>
       </c>
-      <c r="F50" s="22">
-        <v>0</v>
-      </c>
-      <c r="G50" s="7" t="s">
+      <c r="F55" s="22">
+        <v>0</v>
+      </c>
+      <c r="G55" s="7" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="51" spans="2:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B51" s="6" t="s">
+    <row r="56" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B56" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="C51" s="6" t="s">
+      <c r="C56" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="D51" s="6" t="s">
+      <c r="D56" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="E51" s="22">
+      <c r="E56" s="22">
         <v>0.44</v>
       </c>
-      <c r="F51" s="22">
-        <v>0</v>
-      </c>
-      <c r="G51" s="8" t="s">
+      <c r="F56" s="22">
+        <v>0</v>
+      </c>
+      <c r="G56" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="2:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B52" s="6" t="s">
+    <row r="57" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B57" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C52" s="6" t="s">
+      <c r="C57" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D52" s="6" t="s">
+      <c r="D57" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="E52" s="22">
+      <c r="E57" s="22">
         <v>0.37</v>
       </c>
-      <c r="F52" s="22">
-        <v>0</v>
-      </c>
-      <c r="G52" s="8" t="s">
+      <c r="F57" s="22">
+        <v>0</v>
+      </c>
+      <c r="G57" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="2:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B53" s="6" t="s">
+    <row r="58" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B58" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="C53" s="6" t="s">
+      <c r="C58" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="D53" s="6" t="s">
+      <c r="D58" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="E53" s="22">
+      <c r="E58" s="22">
         <v>20000</v>
       </c>
-      <c r="F53" s="22">
-        <v>0</v>
-      </c>
-      <c r="G53" s="8" t="s">
+      <c r="F58" s="22">
+        <v>0</v>
+      </c>
+      <c r="G58" s="8" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="54" spans="2:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B54" s="6" t="s">
+    <row r="59" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B59" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C54" s="6" t="s">
+      <c r="C59" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D54" s="6" t="s">
+      <c r="D59" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="E54" s="9">
+      <c r="E59" s="9">
         <v>0.99</v>
       </c>
-      <c r="F54" s="22">
-        <v>0</v>
-      </c>
-      <c r="G54" s="7" t="s">
+      <c r="F59" s="22">
+        <v>0</v>
+      </c>
+      <c r="G59" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="2:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B55" s="6" t="s">
+    <row r="60" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B60" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="C55" s="6" t="s">
+      <c r="C60" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D55" s="6" t="s">
+      <c r="D60" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="E55" s="9">
+      <c r="E60" s="9">
         <v>0.01</v>
       </c>
-      <c r="F55" s="22">
-        <v>0</v>
-      </c>
-      <c r="G55" s="7" t="s">
+      <c r="F60" s="22">
+        <v>0</v>
+      </c>
+      <c r="G60" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="2:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B56" s="6" t="s">
+    <row r="61" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B61" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="C56" s="6" t="s">
+      <c r="C61" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D56" s="6" t="s">
+      <c r="D61" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="E56" s="9">
+      <c r="E61" s="9">
         <v>25.9</v>
       </c>
-      <c r="F56" s="22">
-        <v>0</v>
-      </c>
-      <c r="G56" s="8" t="s">
+      <c r="F61" s="22">
+        <v>0</v>
+      </c>
+      <c r="G61" s="8" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="57" spans="2:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B57" s="6" t="s">
+    <row r="62" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B62" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="C57" s="6" t="s">
+      <c r="C62" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D57" s="6" t="s">
+      <c r="D62" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="E57" s="37">
+      <c r="E62" s="37">
         <v>1.3300000000000001E-14</v>
       </c>
-      <c r="F57" s="22">
-        <v>0</v>
-      </c>
-      <c r="G57" s="8" t="s">
+      <c r="F62" s="22">
+        <v>0</v>
+      </c>
+      <c r="G62" s="8" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="58" spans="2:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B58" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="D58" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="E58" s="37">
+    <row r="63" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B63" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="E63" s="22">
         <v>1</v>
       </c>
-      <c r="F58" s="22">
-        <v>0</v>
-      </c>
-      <c r="G58" s="8" t="s">
+      <c r="F63" s="22">
+        <v>0</v>
+      </c>
+      <c r="G63" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="59" spans="2:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B59" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="E59" s="22">
-        <v>1</v>
-      </c>
-      <c r="F59" s="22">
-        <v>0</v>
-      </c>
-      <c r="G59" s="8" t="s">
+    <row r="64" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B64" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="E64" s="22">
+        <v>100</v>
+      </c>
+      <c r="F64" s="22">
+        <v>0</v>
+      </c>
+      <c r="G64" s="8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B65" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="E65" s="38" t="s">
+        <v>144</v>
+      </c>
+      <c r="F65" s="39">
+        <v>0</v>
+      </c>
+      <c r="G65" s="8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B66" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="E66" s="38" t="s">
+        <v>145</v>
+      </c>
+      <c r="F66" s="39">
+        <v>0</v>
+      </c>
+      <c r="G66" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="60" spans="2:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B60" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="C60" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="D60" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="E60" s="22">
-        <v>100</v>
-      </c>
-      <c r="F60" s="22">
-        <v>0</v>
-      </c>
-      <c r="G60" s="8" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="61" spans="2:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B61" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="C61" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D61" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="E61" s="38" t="s">
-        <v>144</v>
-      </c>
-      <c r="F61" s="39">
-        <v>0</v>
-      </c>
-      <c r="G61" s="8" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="62" spans="2:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B62" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="C62" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D62" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="E62" s="38" t="s">
-        <v>145</v>
-      </c>
-      <c r="F62" s="39">
-        <v>0</v>
-      </c>
-      <c r="G62" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="63" spans="2:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B63" s="6" t="s">
+    <row r="67" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B67" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="C63" s="6" t="s">
+      <c r="C67" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D63" s="6" t="s">
+      <c r="D67" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="E63" s="9">
+      <c r="E67" s="9">
         <v>0.02</v>
-      </c>
-      <c r="F63" s="22">
-        <v>0</v>
-      </c>
-      <c r="G63" s="8" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="64" spans="2:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B64" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C64" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D64" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="E64" s="22">
-        <v>0.22</v>
-      </c>
-      <c r="F64" s="22">
-        <v>0</v>
-      </c>
-      <c r="G64" s="8" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B65" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C65" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D65" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="E65" s="22">
-        <v>1</v>
-      </c>
-      <c r="F65" s="22">
-        <v>0</v>
-      </c>
-      <c r="G65" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B66" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C66" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D66" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="E66" s="22">
-        <v>0</v>
-      </c>
-      <c r="F66" s="22">
-        <v>0</v>
-      </c>
-      <c r="G66" s="8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B67" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C67" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D67" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="E67" s="33">
-        <v>0</v>
       </c>
       <c r="F67" s="22">
         <v>0</v>
@@ -3770,38 +3770,38 @@
         <v>121</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" ht="15.95" customHeight="1">
       <c r="B68" s="6" t="s">
-        <v>115</v>
+        <v>11</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>116</v>
+        <v>67</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E68" s="22">
-        <v>1.5</v>
+        <v>0.22</v>
       </c>
       <c r="F68" s="22">
         <v>0</v>
       </c>
       <c r="G68" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="15.95" customHeight="1">
       <c r="B69" s="6" t="s">
-        <v>117</v>
+        <v>13</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>118</v>
+        <v>69</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E69" s="22">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="F69" s="22">
         <v>0</v>
@@ -3810,23 +3810,104 @@
         <v>14</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
+    <row r="70" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B70" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="E70" s="22">
+        <v>0</v>
+      </c>
+      <c r="F70" s="22">
+        <v>0</v>
+      </c>
+      <c r="G70" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B71" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="E71" s="33">
+        <v>0</v>
+      </c>
+      <c r="F71" s="22">
+        <v>0</v>
+      </c>
+      <c r="G71" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B72" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="E72" s="22">
+        <v>1.5</v>
+      </c>
+      <c r="F72" s="22">
+        <v>0</v>
+      </c>
+      <c r="G72" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B73" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="E73" s="22">
+        <v>1.5</v>
+      </c>
+      <c r="F73" s="22">
+        <v>0</v>
+      </c>
+      <c r="G73" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="15.95" customHeight="1">
+      <c r="A74" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" spans="1:7" ht="15.95" customHeight="1"/>
+    <row r="76" spans="1:7" ht="15.95" customHeight="1"/>
+    <row r="77" spans="1:7" ht="15.95" customHeight="1"/>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="B44:G44"/>
+  <mergeCells count="8">
+    <mergeCell ref="B49:G49"/>
     <mergeCell ref="B2:G3"/>
     <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B43:G43"/>
+    <mergeCell ref="B37:G37"/>
     <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="B32:G32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="61" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3839,111 +3920,111 @@
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="18.75"/>
   <cols>
     <col min="1" max="1" width="3" style="13" customWidth="1"/>
-    <col min="2" max="2" width="6.1640625" style="13" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="6.125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="14.875" style="14" customWidth="1"/>
     <col min="4" max="4" width="9.5" style="13" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="13"/>
+    <col min="5" max="16384" width="10.875" style="13"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1">
       <c r="A5" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1">
       <c r="A7" s="13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1">
       <c r="A9" s="13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1">
       <c r="A10" s="13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1">
       <c r="A11" s="13" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1">
       <c r="A12" s="13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1">
       <c r="A14" s="13" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1">
       <c r="A15" s="13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1">
       <c r="A16" s="13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" s="13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" s="13" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" s="13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" s="13" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="A22" s="13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23" s="13" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="A24" s="13" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2">
       <c r="A25" s="13" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="A26" s="13" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2">
       <c r="A28" s="13" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2">
       <c r="A29" s="13" t="s">
         <v>40</v>
       </c>
@@ -3951,7 +4032,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2">
       <c r="A30" s="13" t="s">
         <v>42</v>
       </c>
@@ -3959,32 +4040,32 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2">
       <c r="B31" s="13" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2">
       <c r="B32" s="13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4">
       <c r="B33" s="13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4">
       <c r="B34" s="13" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4">
       <c r="B35" s="13" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4">
       <c r="A36" s="18" t="s">
         <v>53</v>
       </c>
@@ -3992,38 +4073,38 @@
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4">
       <c r="B37" s="13" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4">
       <c r="B38" s="13" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4">
       <c r="B39" s="13" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4">
       <c r="B41" s="13" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4">
       <c r="B42" s="13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4">
       <c r="B43" s="13" t="s">
         <v>57</v>
       </c>
       <c r="C43" s="13"/>
     </row>
-    <row r="44" spans="1:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="19.5" thickBot="1">
       <c r="C44" s="15" t="s">
         <v>51</v>
       </c>
@@ -4031,7 +4112,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4">
       <c r="C45" s="14">
         <v>0</v>
       </c>
@@ -4039,7 +4120,7 @@
         <v>11.16</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4">
       <c r="C46" s="14">
         <v>0.1</v>
       </c>
@@ -4047,7 +4128,7 @@
         <v>0.81789999999999996</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4">
       <c r="C47" s="14">
         <v>0.2</v>
       </c>
@@ -4055,7 +4136,7 @@
         <v>0.56440000000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4">
       <c r="C48" s="14">
         <v>0.3</v>
       </c>

</xml_diff>

<commit_message>
Implement GITT processing script
</commit_message>
<xml_diff>
--- a/GEN2_XLSX_CELLDEFS/cellLMO-P2DM.xlsx
+++ b/GEN2_XLSX_CELLDEFS/cellLMO-P2DM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CLiMB\LMB_Toolkit_Latest\GEN2_XLSX_CELLDEFS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC59BE3-29B3-415D-8B07-8661458CD942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D1D55D3-20D2-4D7F-8CDD-20BB6BEE9A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="629" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -545,9 +545,6 @@
     <t>[14.56, 13.21]</t>
   </si>
   <si>
-    <t>[0.2, 0.71307]</t>
-  </si>
-  <si>
     <t>[1.12446, 1.71031]</t>
   </si>
   <si>
@@ -720,6 +717,9 @@
   </si>
   <si>
     <t>V_\mathrm{max}</t>
+  </si>
+  <si>
+    <t>[0.5, 0.5]</t>
   </si>
 </sst>
 </file>
@@ -2605,7 +2605,7 @@
   <dimension ref="A1:G79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B50" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+      <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2702,16 +2702,16 @@
         <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.95" customHeight="1">
@@ -2722,16 +2722,16 @@
         <v>85</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E8" s="19" t="s">
         <v>109</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1">
@@ -2742,7 +2742,7 @@
     </row>
     <row r="10" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
       <c r="B10" s="41" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C10" s="42"/>
       <c r="D10" s="42"/>
@@ -2752,7 +2752,7 @@
     </row>
     <row r="11" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A11" s="32" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>1</v>
@@ -2775,13 +2775,13 @@
     </row>
     <row r="12" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="B12" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="D12" s="6" t="s">
         <v>190</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>191</v>
       </c>
       <c r="E12" s="23">
         <v>0.1</v>
@@ -2790,18 +2790,18 @@
         <v>0</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="B13" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="D13" s="6" t="s">
         <v>194</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>195</v>
       </c>
       <c r="E13" s="40">
         <v>1E-8</v>
@@ -2810,7 +2810,7 @@
         <v>0</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1">
@@ -2881,7 +2881,7 @@
         <v>98</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E18" s="23">
         <v>1000</v>
@@ -2901,7 +2901,7 @@
         <v>19</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E19" s="22">
         <v>0.8</v>
@@ -2921,7 +2921,7 @@
         <v>103</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E20" s="33">
         <v>2.5800000000000002E-9</v>
@@ -2941,7 +2941,7 @@
         <v>106</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E21" s="22">
         <v>0.4</v>
@@ -2961,7 +2961,7 @@
         <v>108</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E22" s="22">
         <v>3</v>
@@ -2975,13 +2975,13 @@
     </row>
     <row r="23" spans="1:7" ht="15.95" customHeight="1">
       <c r="B23" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E23" s="22">
         <v>3</v>
@@ -2995,13 +2995,13 @@
     </row>
     <row r="24" spans="1:7" ht="15.95" customHeight="1">
       <c r="B24" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C24" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>202</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>203</v>
       </c>
       <c r="E24" s="22">
         <v>4.2</v>
@@ -3015,13 +3015,13 @@
     </row>
     <row r="25" spans="1:7" ht="15.95" customHeight="1">
       <c r="B25" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E25" s="22">
         <v>298.14999999999998</v>
@@ -3030,7 +3030,7 @@
         <v>0</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1">
@@ -3080,7 +3080,7 @@
         <v>20</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E29" s="33">
         <v>3.5000000000000002E-8</v>
@@ -3094,13 +3094,13 @@
     </row>
     <row r="30" spans="1:7" ht="15.95" customHeight="1">
       <c r="B30" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C30" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="D30" s="6" t="s">
         <v>161</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>162</v>
       </c>
       <c r="E30" s="33">
         <v>76900</v>
@@ -3120,10 +3120,10 @@
         <v>21</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E31" s="9">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="F31" s="22">
         <v>0</v>
@@ -3140,7 +3140,7 @@
         <v>113</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E32" s="22">
         <v>1</v>
@@ -3160,7 +3160,7 @@
         <v>24</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E33" s="9">
         <v>0.02</v>
@@ -3180,7 +3180,7 @@
         <v>67</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E34" s="22">
         <v>0.19800000000000001</v>
@@ -3200,7 +3200,7 @@
         <v>69</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E35" s="22">
         <v>1</v>
@@ -3220,7 +3220,7 @@
         <v>25</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E36" s="22">
         <v>9.9999999999999995E-7</v>
@@ -3240,7 +3240,7 @@
         <v>66</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E37" s="33">
         <v>0</v>
@@ -3319,7 +3319,7 @@
         <v>126</v>
       </c>
       <c r="D42" s="29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E42" s="30">
         <v>0.21</v>
@@ -3339,7 +3339,7 @@
         <v>118</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E43" s="30">
         <v>1.5</v>
@@ -3418,7 +3418,7 @@
         <v>126</v>
       </c>
       <c r="D48" s="29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E48" s="22">
         <v>0.41</v>
@@ -3438,7 +3438,7 @@
         <v>118</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E49" s="22">
         <v>1.5</v>
@@ -3496,7 +3496,7 @@
         <v>71</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E53" s="21" t="s">
         <v>142</v>
@@ -3516,7 +3516,7 @@
         <v>73</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E54" s="21" t="s">
         <v>143</v>
@@ -3536,10 +3536,10 @@
         <v>75</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E55" s="21" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F55" s="9">
         <v>0</v>
@@ -3576,7 +3576,7 @@
         <v>131</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E57" s="36">
         <v>3.9999999999999998E-6</v>
@@ -3596,7 +3596,7 @@
         <v>133</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E58" s="22">
         <v>0.44</v>
@@ -3616,7 +3616,7 @@
         <v>126</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E59" s="22">
         <v>0.37</v>
@@ -3636,7 +3636,7 @@
         <v>135</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E60" s="22">
         <v>20000</v>
@@ -3656,7 +3656,7 @@
         <v>16</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E61" s="9">
         <v>0.99</v>
@@ -3676,7 +3676,7 @@
         <v>17</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E62" s="9">
         <v>0.01</v>
@@ -3696,7 +3696,7 @@
         <v>18</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E63" s="9">
         <v>25.9</v>
@@ -3716,7 +3716,7 @@
         <v>23</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E64" s="37">
         <v>1.3300000000000001E-14</v>
@@ -3736,7 +3736,7 @@
         <v>68</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E65" s="22">
         <v>1</v>
@@ -3750,13 +3750,13 @@
     </row>
     <row r="66" spans="1:7" ht="15.95" customHeight="1">
       <c r="B66" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="C66" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="C66" s="6" t="s">
+      <c r="D66" s="6" t="s">
         <v>185</v>
-      </c>
-      <c r="D66" s="6" t="s">
-        <v>186</v>
       </c>
       <c r="E66" s="22">
         <v>100</v>
@@ -3765,7 +3765,7 @@
         <v>0</v>
       </c>
       <c r="G66" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="15.95" customHeight="1">
@@ -3776,7 +3776,7 @@
         <v>20</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E67" s="38" t="s">
         <v>144</v>
@@ -3785,7 +3785,7 @@
         <v>0</v>
       </c>
       <c r="G67" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="15.95" customHeight="1">
@@ -3796,10 +3796,10 @@
         <v>21</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E68" s="38" t="s">
-        <v>145</v>
+        <v>203</v>
       </c>
       <c r="F68" s="39">
         <v>0</v>
@@ -3816,7 +3816,7 @@
         <v>24</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E69" s="9">
         <v>0.02</v>
@@ -3836,7 +3836,7 @@
         <v>67</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E70" s="22">
         <v>0.22</v>
@@ -3856,7 +3856,7 @@
         <v>69</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E71" s="22">
         <v>1</v>
@@ -3876,7 +3876,7 @@
         <v>25</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E72" s="22">
         <v>9.9999999999999995E-7</v>
@@ -3896,7 +3896,7 @@
         <v>66</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E73" s="33">
         <v>0</v>
@@ -3916,7 +3916,7 @@
         <v>116</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E74" s="22">
         <v>1.5</v>
@@ -3936,7 +3936,7 @@
         <v>118</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E75" s="22">
         <v>1.5</v>

</xml_diff>

<commit_message>
All TF dc gains stable1
</commit_message>
<xml_diff>
--- a/GEN2_XLSX_CELLDEFS/cellLMO-P2DM.xlsx
+++ b/GEN2_XLSX_CELLDEFS/cellLMO-P2DM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CLiMB\LMB_Toolkit_Latest\GEN2_XLSX_CELLDEFS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D1D55D3-20D2-4D7F-8CDD-20BB6BEE9A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85EE7C53-121A-4BDA-920D-39C1EEB21619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="629" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="629" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="16" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="203">
   <si>
     <t>Code Name</t>
   </si>
@@ -128,16 +128,10 @@
     <t>alpha</t>
   </si>
   <si>
-    <t>Double-layer CPE frequency breakpoint</t>
-  </si>
-  <si>
     <t>Dsref</t>
   </si>
   <si>
     <t>Rf</t>
-  </si>
-  <si>
-    <t>wDL</t>
   </si>
   <si>
     <t>INSTRUCTIONS FOR USING A CELL-PARAMETER-VALUE SPREADSHEET FOR THE PHYSICS-BASED TOOLBOX</t>
@@ -392,9 +386,6 @@
     <t>Sectioning</t>
   </si>
   <si>
-    <t>rad/s</t>
-  </si>
-  <si>
     <t>Current-collector plate area</t>
   </si>
   <si>
@@ -611,9 +602,6 @@
     <t>n_\mathrm{dl}</t>
   </si>
   <si>
-    <t>\omega_\mathrm{dl}</t>
-  </si>
-  <si>
     <t>R_\mathrm{dl}</t>
   </si>
   <si>
@@ -720,6 +708,15 @@
   </si>
   <si>
     <t>[0.5, 0.5]</t>
+  </si>
+  <si>
+    <t>tauDL</t>
+  </si>
+  <si>
+    <t>\tau_\mathrm{dl}</t>
+  </si>
+  <si>
+    <t>Double-layer CPE-integrator time constant</t>
   </si>
 </sst>
 </file>
@@ -2604,8 +2601,8 @@
   </sheetPr>
   <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B50" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E69" sqref="E69"/>
+    <sheetView tabSelected="1" topLeftCell="B53" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2621,22 +2618,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="35.1" hidden="1" customHeight="1" thickBot="1">
       <c r="A1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
@@ -2673,7 +2670,7 @@
     </row>
     <row r="6" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="32" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>1</v>
@@ -2682,13 +2679,13 @@
         <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>2</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>3</v>
@@ -2696,53 +2693,53 @@
     </row>
     <row r="7" spans="1:7" ht="15.95" customHeight="1">
       <c r="B7" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.95" customHeight="1">
       <c r="B8" s="10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
       <c r="B10" s="41" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C10" s="42"/>
       <c r="D10" s="42"/>
@@ -2752,7 +2749,7 @@
     </row>
     <row r="11" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A11" s="32" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>1</v>
@@ -2761,13 +2758,13 @@
         <v>0</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E11" s="11" t="s">
         <v>2</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>3</v>
@@ -2775,13 +2772,13 @@
     </row>
     <row r="12" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="B12" s="5" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E12" s="23">
         <v>0.1</v>
@@ -2790,18 +2787,18 @@
         <v>0</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="B13" s="5" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E13" s="40">
         <v>1E-8</v>
@@ -2810,12 +2807,12 @@
         <v>0</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G14" s="20"/>
     </row>
@@ -2831,7 +2828,7 @@
     </row>
     <row r="16" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A16" s="32" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>1</v>
@@ -2840,13 +2837,13 @@
         <v>0</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>2</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>3</v>
@@ -2854,13 +2851,13 @@
     </row>
     <row r="17" spans="1:7" ht="15.95" customHeight="1">
       <c r="B17" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E17" s="23">
         <f>0.0064</f>
@@ -2870,18 +2867,18 @@
         <v>0</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.95" customHeight="1">
       <c r="B18" s="5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E18" s="23">
         <v>1000</v>
@@ -2890,18 +2887,18 @@
         <v>0</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.95" customHeight="1">
       <c r="B19" s="6" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E19" s="22">
         <v>0.8</v>
@@ -2910,18 +2907,18 @@
         <v>0</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.95" customHeight="1">
       <c r="B20" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E20" s="33">
         <v>2.5800000000000002E-9</v>
@@ -2930,18 +2927,18 @@
         <v>0</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.95" customHeight="1">
       <c r="B21" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E21" s="22">
         <v>0.4</v>
@@ -2955,13 +2952,13 @@
     </row>
     <row r="22" spans="1:7" ht="15.95" customHeight="1">
       <c r="B22" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E22" s="22">
         <v>3</v>
@@ -2975,13 +2972,13 @@
     </row>
     <row r="23" spans="1:7" ht="15.95" customHeight="1">
       <c r="B23" s="6" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="E23" s="22">
         <v>3</v>
@@ -2995,13 +2992,13 @@
     </row>
     <row r="24" spans="1:7" ht="15.95" customHeight="1">
       <c r="B24" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>198</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>202</v>
       </c>
       <c r="E24" s="22">
         <v>4.2</v>
@@ -3015,13 +3012,13 @@
     </row>
     <row r="25" spans="1:7" ht="15.95" customHeight="1">
       <c r="B25" s="6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E25" s="22">
         <v>298.14999999999998</v>
@@ -3030,12 +3027,12 @@
         <v>0</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A26" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G26" s="20"/>
     </row>
@@ -3051,7 +3048,7 @@
     </row>
     <row r="28" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A28" s="32" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>1</v>
@@ -3060,13 +3057,13 @@
         <v>0</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E28" s="11" t="s">
         <v>2</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>3</v>
@@ -3074,13 +3071,13 @@
     </row>
     <row r="29" spans="1:7" ht="15.95" customHeight="1">
       <c r="B29" s="6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>20</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E29" s="33">
         <v>3.5000000000000002E-8</v>
@@ -3089,18 +3086,18 @@
         <v>0</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.95" customHeight="1">
       <c r="B30" s="6" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E30" s="33">
         <v>76900</v>
@@ -3109,18 +3106,18 @@
         <v>0</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15.95" customHeight="1">
       <c r="B31" s="6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E31" s="9">
         <v>0.5</v>
@@ -3134,13 +3131,13 @@
     </row>
     <row r="32" spans="1:7" ht="15.95" customHeight="1">
       <c r="B32" s="6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E32" s="22">
         <v>1</v>
@@ -3149,18 +3146,18 @@
         <v>0</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15.95" customHeight="1">
       <c r="B33" s="6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E33" s="9">
         <v>0.02</v>
@@ -3169,7 +3166,7 @@
         <v>0</v>
       </c>
       <c r="G33" s="34" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15.95" customHeight="1">
@@ -3177,10 +3174,10 @@
         <v>11</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E34" s="22">
         <v>0.19800000000000001</v>
@@ -3189,7 +3186,7 @@
         <v>0</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.95" customHeight="1">
@@ -3197,10 +3194,10 @@
         <v>13</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E35" s="22">
         <v>1</v>
@@ -3214,22 +3211,22 @@
     </row>
     <row r="36" spans="1:7" ht="15.95" customHeight="1">
       <c r="B36" s="6" t="s">
-        <v>22</v>
+        <v>202</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>25</v>
+        <v>200</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="E36" s="22">
-        <v>9.9999999999999995E-7</v>
+        <v>201</v>
+      </c>
+      <c r="E36" s="33">
+        <v>1000</v>
       </c>
       <c r="F36" s="22">
         <v>0</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>94</v>
+        <v>182</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.95" customHeight="1">
@@ -3237,10 +3234,10 @@
         <v>12</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E37" s="33">
         <v>0</v>
@@ -3249,18 +3246,18 @@
         <v>0</v>
       </c>
       <c r="G37" s="34" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A38" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G38" s="20"/>
     </row>
     <row r="39" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
       <c r="B39" s="50" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C39" s="51"/>
       <c r="D39" s="51"/>
@@ -3270,7 +3267,7 @@
     </row>
     <row r="40" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A40" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B40" s="24" t="s">
         <v>1</v>
@@ -3279,13 +3276,13 @@
         <v>0</v>
       </c>
       <c r="D40" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E40" s="25" t="s">
         <v>2</v>
       </c>
       <c r="F40" s="26" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G40" s="27" t="s">
         <v>3</v>
@@ -3293,13 +3290,13 @@
     </row>
     <row r="41" spans="1:7" ht="15.95" customHeight="1">
       <c r="B41" s="28" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C41" s="29" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D41" s="29" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E41" s="35">
         <v>5.0000000000000004E-6</v>
@@ -3308,18 +3305,18 @@
         <v>0</v>
       </c>
       <c r="G41" s="31" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15.95" customHeight="1">
       <c r="B42" s="28" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C42" s="29" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D42" s="29" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E42" s="30">
         <v>0.21</v>
@@ -3333,13 +3330,13 @@
     </row>
     <row r="43" spans="1:7" ht="15.95" customHeight="1">
       <c r="B43" s="28" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C43" s="29" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E43" s="30">
         <v>1.5</v>
@@ -3353,13 +3350,13 @@
     </row>
     <row r="44" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A44" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G44" s="20"/>
     </row>
     <row r="45" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
       <c r="B45" s="41" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C45" s="42"/>
       <c r="D45" s="42"/>
@@ -3369,7 +3366,7 @@
     </row>
     <row r="46" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A46" s="32" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B46" s="11" t="s">
         <v>1</v>
@@ -3378,13 +3375,13 @@
         <v>0</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E46" s="11" t="s">
         <v>2</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G46" s="3" t="s">
         <v>3</v>
@@ -3392,13 +3389,13 @@
     </row>
     <row r="47" spans="1:7" ht="15.95" customHeight="1">
       <c r="B47" s="6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D47" s="29" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E47" s="36">
         <v>2.5000000000000001E-5</v>
@@ -3407,18 +3404,18 @@
         <v>0</v>
       </c>
       <c r="G47" s="8" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="15.95" customHeight="1">
       <c r="B48" s="6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D48" s="29" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E48" s="22">
         <v>0.41</v>
@@ -3432,13 +3429,13 @@
     </row>
     <row r="49" spans="1:7" ht="15.95" customHeight="1">
       <c r="B49" s="6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E49" s="22">
         <v>1.5</v>
@@ -3452,7 +3449,7 @@
     </row>
     <row r="50" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A50" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
@@ -3467,7 +3464,7 @@
     </row>
     <row r="52" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A52" s="32" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B52" s="11" t="s">
         <v>1</v>
@@ -3476,13 +3473,13 @@
         <v>0</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E52" s="11" t="s">
         <v>2</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G52" s="3" t="s">
         <v>3</v>
@@ -3490,16 +3487,16 @@
     </row>
     <row r="53" spans="1:7" ht="15.95" customHeight="1">
       <c r="B53" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E53" s="21" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F53" s="9">
         <v>0</v>
@@ -3510,16 +3507,16 @@
     </row>
     <row r="54" spans="1:7" ht="15.95" customHeight="1">
       <c r="B54" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E54" s="21" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F54" s="9">
         <v>0</v>
@@ -3530,16 +3527,16 @@
     </row>
     <row r="55" spans="1:7" ht="15.95" customHeight="1">
       <c r="B55" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E55" s="21" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F55" s="9">
         <v>0</v>
@@ -3550,13 +3547,13 @@
     </row>
     <row r="56" spans="1:7" ht="15.95" customHeight="1">
       <c r="B56" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E56" s="36">
         <v>2.0000000000000001E-4</v>
@@ -3565,18 +3562,18 @@
         <v>0</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="15.95" customHeight="1">
       <c r="B57" s="6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E57" s="36">
         <v>3.9999999999999998E-6</v>
@@ -3585,18 +3582,18 @@
         <v>0</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="15.95" customHeight="1">
       <c r="B58" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E58" s="22">
         <v>0.44</v>
@@ -3610,13 +3607,13 @@
     </row>
     <row r="59" spans="1:7" ht="15.95" customHeight="1">
       <c r="B59" s="6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E59" s="22">
         <v>0.37</v>
@@ -3630,13 +3627,13 @@
     </row>
     <row r="60" spans="1:7" ht="15.95" customHeight="1">
       <c r="B60" s="6" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E60" s="22">
         <v>20000</v>
@@ -3645,18 +3642,18 @@
         <v>0</v>
       </c>
       <c r="G60" s="8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="15.95" customHeight="1">
       <c r="B61" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E61" s="9">
         <v>0.99</v>
@@ -3670,13 +3667,13 @@
     </row>
     <row r="62" spans="1:7" ht="15.95" customHeight="1">
       <c r="B62" s="6" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C62" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E62" s="9">
         <v>0.01</v>
@@ -3690,13 +3687,13 @@
     </row>
     <row r="63" spans="1:7" ht="15.95" customHeight="1">
       <c r="B63" s="6" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C63" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E63" s="9">
         <v>25.9</v>
@@ -3705,18 +3702,18 @@
         <v>0</v>
       </c>
       <c r="G63" s="8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="15.95" customHeight="1">
       <c r="B64" s="6" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E64" s="37">
         <v>1.3300000000000001E-14</v>
@@ -3725,7 +3722,7 @@
         <v>0</v>
       </c>
       <c r="G64" s="8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="15.95" customHeight="1">
@@ -3733,13 +3730,13 @@
         <v>15</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E65" s="22">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="F65" s="22">
         <v>0</v>
@@ -3750,13 +3747,13 @@
     </row>
     <row r="66" spans="1:7" ht="15.95" customHeight="1">
       <c r="B66" s="6" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E66" s="22">
         <v>100</v>
@@ -3765,41 +3762,41 @@
         <v>0</v>
       </c>
       <c r="G66" s="8" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="15.95" customHeight="1">
       <c r="B67" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C67" s="6" t="s">
         <v>20</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E67" s="38" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F67" s="39">
         <v>0</v>
       </c>
       <c r="G67" s="8" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="15.95" customHeight="1">
       <c r="B68" s="6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E68" s="38" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F68" s="39">
         <v>0</v>
@@ -3810,13 +3807,13 @@
     </row>
     <row r="69" spans="1:7" ht="15.95" customHeight="1">
       <c r="B69" s="6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E69" s="9">
         <v>0.02</v>
@@ -3825,7 +3822,7 @@
         <v>0</v>
       </c>
       <c r="G69" s="8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="15.95" customHeight="1">
@@ -3833,19 +3830,19 @@
         <v>11</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E70" s="22">
-        <v>0.22</v>
+        <v>10</v>
       </c>
       <c r="F70" s="22">
         <v>0</v>
       </c>
       <c r="G70" s="8" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="15.95" customHeight="1">
@@ -3853,13 +3850,13 @@
         <v>13</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E71" s="22">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F71" s="22">
         <v>0</v>
@@ -3870,22 +3867,22 @@
     </row>
     <row r="72" spans="1:7" ht="15.95" customHeight="1">
       <c r="B72" s="6" t="s">
-        <v>22</v>
+        <v>202</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>25</v>
+        <v>200</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="E72" s="22">
-        <v>9.9999999999999995E-7</v>
+        <v>201</v>
+      </c>
+      <c r="E72" s="33">
+        <v>100</v>
       </c>
       <c r="F72" s="22">
         <v>0</v>
       </c>
       <c r="G72" s="8" t="s">
-        <v>94</v>
+        <v>182</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="15.95" customHeight="1">
@@ -3893,10 +3890,10 @@
         <v>12</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E73" s="33">
         <v>0</v>
@@ -3905,18 +3902,18 @@
         <v>0</v>
       </c>
       <c r="G73" s="8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="15.95" customHeight="1">
       <c r="B74" s="6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E74" s="22">
         <v>1.5</v>
@@ -3930,13 +3927,13 @@
     </row>
     <row r="75" spans="1:7" ht="15.95" customHeight="1">
       <c r="B75" s="6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E75" s="22">
         <v>1.5</v>
@@ -3950,7 +3947,7 @@
     </row>
     <row r="76" spans="1:7" ht="15.95" customHeight="1">
       <c r="A76" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="15.95" customHeight="1"/>
@@ -3989,185 +3986,185 @@
   <sheetData>
     <row r="5" spans="1:1">
       <c r="A5" s="12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="B31" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="B32" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="B33" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="B34" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="B35" s="13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="B37" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="B38" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="B39" s="13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="B41" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="B42" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="B43" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C43" s="13"/>
     </row>
     <row r="44" spans="1:4" ht="19.5" thickBot="1">
       <c r="C44" s="15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:4">

</xml_diff>

<commit_message>
TFs stable, RPT development
</commit_message>
<xml_diff>
--- a/GEN2_XLSX_CELLDEFS/cellLMO-P2DM.xlsx
+++ b/GEN2_XLSX_CELLDEFS/cellLMO-P2DM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CLiMB\LMB_Toolkit_Latest\GEN2_XLSX_CELLDEFS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85EE7C53-121A-4BDA-920D-39C1EEB21619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7762E817-FE4C-4580-84F3-E5FC9AE032BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="629" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="629" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="16" r:id="rId1"/>
@@ -2601,8 +2601,8 @@
   </sheetPr>
   <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B53" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+    <sheetView tabSelected="1" topLeftCell="B62" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E79" sqref="E79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3736,7 +3736,7 @@
         <v>178</v>
       </c>
       <c r="E65" s="22">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="F65" s="22">
         <v>0</v>
@@ -3836,7 +3836,7 @@
         <v>162</v>
       </c>
       <c r="E70" s="22">
-        <v>10</v>
+        <v>0.22</v>
       </c>
       <c r="F70" s="22">
         <v>0</v>
@@ -3856,7 +3856,7 @@
         <v>163</v>
       </c>
       <c r="E71" s="22">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F71" s="22">
         <v>0</v>
@@ -3896,7 +3896,7 @@
         <v>164</v>
       </c>
       <c r="E73" s="33">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="F73" s="22">
         <v>0</v>

</xml_diff>

<commit_message>
prepare to release to CMI
</commit_message>
<xml_diff>
--- a/GEN2_XLSX_CELLDEFS/cellLMO-P2DM.xlsx
+++ b/GEN2_XLSX_CELLDEFS/cellLMO-P2DM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CLiMB\LMB_Toolkit_Latest\GEN2_XLSX_CELLDEFS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7762E817-FE4C-4580-84F3-E5FC9AE032BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52506396-0AF0-49C9-ADA6-C22A2BD7BA0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="629" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="629" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="16" r:id="rId1"/>
@@ -2601,8 +2601,8 @@
   </sheetPr>
   <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B62" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E79" sqref="E79"/>
+    <sheetView tabSelected="1" topLeftCell="B14" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2981,7 +2981,7 @@
         <v>195</v>
       </c>
       <c r="E23" s="22">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="F23" s="22">
         <v>0</v>

</xml_diff>

<commit_message>
TF regression validation final
</commit_message>
<xml_diff>
--- a/GEN2_XLSX_CELLDEFS/cellLMO-P2DM.xlsx
+++ b/GEN2_XLSX_CELLDEFS/cellLMO-P2DM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uccsoffice365-my.sharepoint.com/personal/whileman_uccs_edu/Documents/MasterThesis/WesH-MasterThesis/assets/GEN2_XLSX_CELLDEFS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{52506396-0AF0-49C9-ADA6-C22A2BD7BA0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C04BA287-6106-5545-BF7B-4E8D325AD7B2}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{52506396-0AF0-49C9-ADA6-C22A2BD7BA0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7409A5E1-0993-E948-8094-13C45C27EAD5}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30520" windowHeight="16100" tabRatio="629" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1880" yWindow="1460" windowWidth="30520" windowHeight="16100" tabRatio="629" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="16" r:id="rId1"/>
@@ -2274,6 +2274,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2601,8 +2605,8 @@
   </sheetPr>
   <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B18" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="B52" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3756,7 +3760,7 @@
         <v>181</v>
       </c>
       <c r="E66" s="22">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F66" s="22">
         <v>0</v>
@@ -3876,7 +3880,7 @@
         <v>201</v>
       </c>
       <c r="E72" s="33">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="F72" s="22">
         <v>0</v>

</xml_diff>